<commit_message>
Update calculation rules for tax deduction
</commit_message>
<xml_diff>
--- a/documentation/Calculate Sheet.xlsx
+++ b/documentation/Calculate Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23780" windowHeight="13660" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23780" windowHeight="13660"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate sheet (PRM)" sheetId="9" r:id="rId1"/>
@@ -1965,11 +1965,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1980,17 +1977,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2001,13 +2004,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2294,7 +2294,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2304,8 +2304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2373,17 +2373,17 @@
       </c>
       <c r="B5" s="57"/>
       <c r="C5" s="61">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="D5" s="62" t="s">
         <v>411</v>
       </c>
       <c r="E5" s="56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="56">
-        <f>IF(E5=12,0.09,(IF(E5=6,0.52,IF(E5=3,0.27,1))))</f>
-        <v>1</v>
+        <f>IF(E5=12,0.09,(IF(E5=2,0.52,IF(E5=4,0.27,1))))</f>
+        <v>0.52</v>
       </c>
       <c r="G5" s="56">
         <v>308</v>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="C6" s="61">
         <f>(C5*G5/1000)*F5</f>
-        <v>30800</v>
+        <v>160160</v>
       </c>
       <c r="O6" s="56">
         <v>12.423</v>
@@ -2425,17 +2425,17 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="14.25" customHeight="1">
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="86" t="s">
         <v>350</v>
       </c>
-      <c r="D8" s="89" t="s">
+      <c r="D8" s="88" t="s">
         <v>386</v>
       </c>
-      <c r="E8" s="92" t="s">
+      <c r="E8" s="89" t="s">
         <v>244</v>
       </c>
-      <c r="F8" s="92"/>
-      <c r="G8" s="92"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
       <c r="O8" s="56">
         <v>12.622999999999999</v>
       </c>
@@ -2445,8 +2445,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="30">
-      <c r="C9" s="88"/>
-      <c r="D9" s="89"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="88"/>
       <c r="E9" s="6" t="s">
         <v>383</v>
       </c>
@@ -2465,7 +2465,7 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="90" t="s">
         <v>387</v>
       </c>
       <c r="C10" s="7">
@@ -2473,19 +2473,19 @@
       </c>
       <c r="D10" s="29">
         <f>$C$5*20/1000</f>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E10" s="45">
         <f>($D$10+0)+((0*20)/1000)</f>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="F10" s="29">
         <f>(E10+0)+((0*40)/1000)</f>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="G10" s="29">
         <f>(D10+0)+((0*45)/1000)</f>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="J10" s="63"/>
       <c r="K10" s="63"/>
@@ -2500,25 +2500,25 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="B11" s="91"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="7">
         <v>2</v>
       </c>
       <c r="D11" s="29">
         <f t="shared" ref="D11:D18" si="1">$C$5*20/1000</f>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E11" s="46">
         <f>(D11+E10)+((E10*20)/1000)</f>
-        <v>4040</v>
+        <v>40400</v>
       </c>
       <c r="F11" s="29">
         <f>(D11+F10)+((F10*40)/1000)</f>
-        <v>4080</v>
+        <v>40800</v>
       </c>
       <c r="G11" s="29">
         <f>(D11+G10)+((G10*45)/1000)</f>
-        <v>4090</v>
+        <v>40900</v>
       </c>
       <c r="J11" s="63"/>
       <c r="K11" s="63"/>
@@ -2533,25 +2533,25 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="B12" s="91"/>
+      <c r="B12" s="90"/>
       <c r="C12" s="7">
         <v>3</v>
       </c>
       <c r="D12" s="29">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E12" s="46">
         <f>(D12+E11)+((E11*20)/1000)</f>
-        <v>6120.8</v>
+        <v>61208</v>
       </c>
       <c r="F12" s="29">
         <f t="shared" ref="F12:F19" si="2">(D12+F11)+((F11*40)/1000)</f>
-        <v>6243.2</v>
+        <v>62432</v>
       </c>
       <c r="G12" s="29">
         <f t="shared" ref="G12:G19" si="3">(D12+G11)+((G11*45)/1000)</f>
-        <v>6274.05</v>
+        <v>62740.5</v>
       </c>
       <c r="J12" s="63"/>
       <c r="K12" s="63"/>
@@ -2559,25 +2559,25 @@
       <c r="M12" s="63"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="B13" s="91"/>
+      <c r="B13" s="90"/>
       <c r="C13" s="7">
         <v>4</v>
       </c>
       <c r="D13" s="29">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E13" s="46">
         <f>(D13+E12)+((E12*20)/1000)</f>
-        <v>8243.2160000000003</v>
+        <v>82432.160000000003</v>
       </c>
       <c r="F13" s="29">
         <f t="shared" si="2"/>
-        <v>8492.9279999999999</v>
+        <v>84929.279999999999</v>
       </c>
       <c r="G13" s="29">
         <f t="shared" si="3"/>
-        <v>8556.3822499999987</v>
+        <v>85563.822499999995</v>
       </c>
       <c r="J13" s="63"/>
       <c r="K13" s="63"/>
@@ -2585,25 +2585,25 @@
       <c r="M13" s="63"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="B14" s="91"/>
+      <c r="B14" s="90"/>
       <c r="C14" s="7">
         <v>5</v>
       </c>
       <c r="D14" s="29">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E14" s="46">
         <f t="shared" ref="E14:E17" si="4">(D14+E13)+((E13*20)/1000)</f>
-        <v>10408.080320000001</v>
+        <v>104080.80320000001</v>
       </c>
       <c r="F14" s="29">
         <f t="shared" si="2"/>
-        <v>10832.645119999999</v>
+        <v>108326.4512</v>
       </c>
       <c r="G14" s="29">
         <f t="shared" si="3"/>
-        <v>10941.419451249998</v>
+        <v>109414.19451249999</v>
       </c>
       <c r="J14" s="63"/>
       <c r="K14" s="63"/>
@@ -2611,25 +2611,25 @@
       <c r="M14" s="63"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="B15" s="91"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="7">
         <v>6</v>
       </c>
       <c r="D15" s="29">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E15" s="46">
         <f t="shared" si="4"/>
-        <v>12616.241926400002</v>
+        <v>126162.41926400001</v>
       </c>
       <c r="F15" s="29">
         <f t="shared" si="2"/>
-        <v>13265.950924799999</v>
+        <v>132659.50924799999</v>
       </c>
       <c r="G15" s="29">
         <f t="shared" si="3"/>
-        <v>13433.783326556248</v>
+        <v>134337.83326556248</v>
       </c>
       <c r="J15" s="63"/>
       <c r="K15" s="63"/>
@@ -2637,25 +2637,25 @@
       <c r="M15" s="63"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="B16" s="91"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="7">
         <v>7</v>
       </c>
       <c r="D16" s="29">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E16" s="46">
         <f t="shared" si="4"/>
-        <v>14868.566764928002</v>
+        <v>148685.66764928002</v>
       </c>
       <c r="F16" s="29">
         <f t="shared" si="2"/>
-        <v>15796.588961792</v>
+        <v>157965.88961791998</v>
       </c>
       <c r="G16" s="29">
         <f t="shared" si="3"/>
-        <v>16038.303576251279</v>
+        <v>160383.03576251279</v>
       </c>
       <c r="J16" s="63"/>
       <c r="K16" s="63"/>
@@ -2663,25 +2663,25 @@
       <c r="M16" s="63"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17" s="91"/>
+      <c r="B17" s="90"/>
       <c r="C17" s="7">
         <v>8</v>
       </c>
       <c r="D17" s="29">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E17" s="46">
         <f t="shared" si="4"/>
-        <v>17165.938100226562</v>
+        <v>171659.38100226561</v>
       </c>
       <c r="F17" s="29">
         <f t="shared" si="2"/>
-        <v>18428.45252026368</v>
+        <v>184284.52520263678</v>
       </c>
       <c r="G17" s="29">
         <f t="shared" si="3"/>
-        <v>18760.027237182589</v>
+        <v>187600.27237182588</v>
       </c>
       <c r="J17" s="63"/>
       <c r="K17" s="63"/>
@@ -2691,25 +2691,25 @@
       <c r="O17" s="64"/>
     </row>
     <row r="18" spans="2:15">
-      <c r="B18" s="91"/>
+      <c r="B18" s="90"/>
       <c r="C18" s="7">
         <v>9</v>
       </c>
       <c r="D18" s="29">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E18" s="46">
         <f>(D18+E17)+((E17*20)/1000)</f>
-        <v>19509.256862231094</v>
+        <v>195092.56862231094</v>
       </c>
       <c r="F18" s="29">
         <f t="shared" si="2"/>
-        <v>21165.590621074225</v>
+        <v>211655.90621074225</v>
       </c>
       <c r="G18" s="29">
         <f t="shared" si="3"/>
-        <v>21604.228462855805</v>
+        <v>216042.28462855803</v>
       </c>
       <c r="J18" s="63"/>
       <c r="K18" s="63"/>
@@ -2717,25 +2717,25 @@
       <c r="M18" s="63"/>
     </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="91"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="7">
         <v>10</v>
       </c>
       <c r="D19" s="29">
         <f>$C$5*1820/1000</f>
-        <v>182000</v>
+        <v>1820000</v>
       </c>
       <c r="E19" s="46">
         <f>(D19+E18)+((E18*20)/1000)</f>
-        <v>201899.4419994757</v>
+        <v>2018994.419994757</v>
       </c>
       <c r="F19" s="29">
         <f t="shared" si="2"/>
-        <v>204012.21424591719</v>
+        <v>2040122.1424591718</v>
       </c>
       <c r="G19" s="29">
         <f t="shared" si="3"/>
-        <v>204576.41874368431</v>
+        <v>2045764.1874368431</v>
       </c>
       <c r="J19" s="63"/>
       <c r="K19" s="63"/>
@@ -2748,35 +2748,35 @@
       </c>
       <c r="D20" s="66">
         <f>SUM(D10:D19)</f>
-        <v>200000</v>
+        <v>2000000</v>
       </c>
       <c r="E20" s="67">
         <f>E19</f>
-        <v>201899.4419994757</v>
+        <v>2018994.419994757</v>
       </c>
       <c r="F20" s="68">
         <f>F19</f>
-        <v>204012.21424591719</v>
+        <v>2040122.1424591718</v>
       </c>
       <c r="G20" s="68">
         <f>G19</f>
-        <v>204576.41874368431</v>
+        <v>2045764.1874368431</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="14.25" customHeight="1">
-      <c r="D23" s="92" t="s">
+      <c r="D23" s="89" t="s">
         <v>352</v>
       </c>
-      <c r="E23" s="92"/>
-      <c r="F23" s="92"/>
-      <c r="G23" s="92"/>
-      <c r="I23" s="93" t="s">
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="I23" s="85" t="s">
         <v>389</v>
       </c>
-      <c r="J23" s="93"/>
-      <c r="K23" s="93"/>
-      <c r="L23" s="93"/>
-      <c r="M23" s="93"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="85"/>
+      <c r="M23" s="85"/>
     </row>
     <row r="24" spans="2:15" ht="30">
       <c r="C24" s="7" t="s">
@@ -2907,7 +2907,7 @@
       <c r="M30" s="69"/>
     </row>
     <row r="31" spans="2:15" ht="14.25" customHeight="1">
-      <c r="B31" s="85" t="s">
+      <c r="B31" s="91" t="s">
         <v>388</v>
       </c>
       <c r="C31" s="7">
@@ -2915,19 +2915,19 @@
       </c>
       <c r="D31" s="9">
         <f>($C$5*1.5)/100</f>
-        <v>1500</v>
+        <v>15000</v>
       </c>
       <c r="E31" s="9">
         <f>(D31+0)+(0*4/100)</f>
-        <v>1500</v>
+        <v>15000</v>
       </c>
       <c r="F31" s="9">
         <f>($C$5*1.8)/100</f>
-        <v>1800</v>
+        <v>18000</v>
       </c>
       <c r="G31" s="9">
         <f>(F31+0)+(0*4.5/100)</f>
-        <v>1800</v>
+        <v>18000</v>
       </c>
       <c r="I31" s="7">
         <v>7</v>
@@ -2946,25 +2946,25 @@
       </c>
     </row>
     <row r="32" spans="2:15">
-      <c r="B32" s="86"/>
+      <c r="B32" s="92"/>
       <c r="C32" s="7">
         <v>8</v>
       </c>
       <c r="D32" s="9">
         <f t="shared" ref="D32:D33" si="5">($C$5*1.5)/100</f>
-        <v>1500</v>
+        <v>15000</v>
       </c>
       <c r="E32" s="35">
         <f>(D32+E31)+(E31*4/100)</f>
-        <v>3060</v>
+        <v>30600</v>
       </c>
       <c r="F32" s="9">
         <f>($C$5*1.8)/100</f>
-        <v>1800</v>
+        <v>18000</v>
       </c>
       <c r="G32" s="9">
         <f>(F32+G31)+(G31*4.5/100)</f>
-        <v>3681</v>
+        <v>36810</v>
       </c>
       <c r="I32" s="7">
         <v>8</v>
@@ -2983,25 +2983,25 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="86"/>
+      <c r="B33" s="92"/>
       <c r="C33" s="7">
         <v>9</v>
       </c>
       <c r="D33" s="9">
         <f t="shared" si="5"/>
-        <v>1500</v>
+        <v>15000</v>
       </c>
       <c r="E33" s="35">
         <f t="shared" ref="E33:E34" si="6">(D33+E32)+(E32*4/100)</f>
-        <v>4682.3999999999996</v>
+        <v>46824</v>
       </c>
       <c r="F33" s="9">
         <f>($C$5*1.8)/100</f>
-        <v>1800</v>
+        <v>18000</v>
       </c>
       <c r="G33" s="9">
         <f t="shared" ref="G33:G34" si="7">(F33+G32)+(G32*4.5/100)</f>
-        <v>5646.6450000000004</v>
+        <v>56466.45</v>
       </c>
       <c r="I33" s="7">
         <v>9</v>
@@ -3020,25 +3020,25 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="86"/>
+      <c r="B34" s="92"/>
       <c r="C34" s="7">
         <v>10</v>
       </c>
       <c r="D34" s="9">
         <f>($C$5*16.5)/100</f>
-        <v>16500</v>
+        <v>165000</v>
       </c>
       <c r="E34" s="35">
         <f t="shared" si="6"/>
-        <v>21369.696</v>
+        <v>213696.96</v>
       </c>
       <c r="F34" s="9">
         <f>($C$5*19.8)/100</f>
-        <v>19800</v>
+        <v>198000</v>
       </c>
       <c r="G34" s="9">
         <f t="shared" si="7"/>
-        <v>25700.744025</v>
+        <v>257007.44025000001</v>
       </c>
       <c r="I34" s="7">
         <v>10</v>
@@ -3057,42 +3057,42 @@
       </c>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="86"/>
+      <c r="B35" s="92"/>
       <c r="C35" s="69"/>
       <c r="D35" s="66">
         <f>SUM(D25:D34)</f>
-        <v>21000</v>
+        <v>210000</v>
       </c>
       <c r="E35" s="71">
         <f>E34</f>
-        <v>21369.696</v>
+        <v>213696.96</v>
       </c>
       <c r="F35" s="66">
         <f>SUM(F25:F34)</f>
-        <v>25200</v>
+        <v>252000</v>
       </c>
       <c r="G35" s="71">
         <f>G34</f>
-        <v>25700.744025</v>
+        <v>257007.44025000001</v>
       </c>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="86"/>
+      <c r="B36" s="92"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="C38" s="87" t="s">
+      <c r="C38" s="86" t="s">
         <v>350</v>
       </c>
-      <c r="D38" s="89"/>
-      <c r="E38" s="90" t="s">
+      <c r="D38" s="88"/>
+      <c r="E38" s="93" t="s">
         <v>355</v>
       </c>
-      <c r="F38" s="90"/>
-      <c r="G38" s="90"/>
+      <c r="F38" s="93"/>
+      <c r="G38" s="93"/>
     </row>
     <row r="39" spans="2:13" ht="30">
-      <c r="C39" s="88"/>
-      <c r="D39" s="89"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="88"/>
       <c r="E39" s="6" t="s">
         <v>356</v>
       </c>
@@ -3104,7 +3104,7 @@
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="91" t="s">
+      <c r="B40" s="90" t="s">
         <v>359</v>
       </c>
       <c r="C40" s="7">
@@ -3113,186 +3113,186 @@
       <c r="D40" s="9"/>
       <c r="E40" s="9">
         <f>E10</f>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="F40" s="35">
         <f>F10+E25</f>
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="G40" s="35">
         <f>G10+G25</f>
-        <v>2000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="91"/>
+      <c r="B41" s="90"/>
       <c r="C41" s="7">
         <v>2</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9">
         <f t="shared" ref="E41:E48" si="8">E11</f>
-        <v>4040</v>
+        <v>40400</v>
       </c>
       <c r="F41" s="35">
         <f t="shared" ref="F41:F49" si="9">F11+E26</f>
-        <v>4080</v>
+        <v>40800</v>
       </c>
       <c r="G41" s="35">
         <f t="shared" ref="G41:G49" si="10">G11+G26</f>
-        <v>4090</v>
+        <v>40900</v>
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="91"/>
+      <c r="B42" s="90"/>
       <c r="C42" s="7">
         <v>3</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9">
         <f t="shared" si="8"/>
-        <v>6120.8</v>
+        <v>61208</v>
       </c>
       <c r="F42" s="35">
         <f t="shared" si="9"/>
-        <v>6243.2</v>
+        <v>62432</v>
       </c>
       <c r="G42" s="35">
         <f t="shared" si="10"/>
-        <v>6274.05</v>
+        <v>62740.5</v>
       </c>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="91"/>
+      <c r="B43" s="90"/>
       <c r="C43" s="7">
         <v>4</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9">
         <f t="shared" si="8"/>
-        <v>8243.2160000000003</v>
+        <v>82432.160000000003</v>
       </c>
       <c r="F43" s="35">
         <f t="shared" si="9"/>
-        <v>8492.9279999999999</v>
+        <v>84929.279999999999</v>
       </c>
       <c r="G43" s="35">
         <f t="shared" si="10"/>
-        <v>8556.3822499999987</v>
+        <v>85563.822499999995</v>
       </c>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="91"/>
+      <c r="B44" s="90"/>
       <c r="C44" s="7">
         <v>5</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9">
         <f t="shared" si="8"/>
-        <v>10408.080320000001</v>
+        <v>104080.80320000001</v>
       </c>
       <c r="F44" s="35">
         <f t="shared" si="9"/>
-        <v>10832.645119999999</v>
+        <v>108326.4512</v>
       </c>
       <c r="G44" s="35">
         <f t="shared" si="10"/>
-        <v>10941.419451249998</v>
+        <v>109414.19451249999</v>
       </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="91"/>
+      <c r="B45" s="90"/>
       <c r="C45" s="7">
         <v>6</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9">
         <f t="shared" si="8"/>
-        <v>12616.241926400002</v>
+        <v>126162.41926400001</v>
       </c>
       <c r="F45" s="35">
         <f t="shared" si="9"/>
-        <v>13265.950924799999</v>
+        <v>132659.50924799999</v>
       </c>
       <c r="G45" s="35">
         <f t="shared" si="10"/>
-        <v>13433.783326556248</v>
+        <v>134337.83326556248</v>
       </c>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="91"/>
+      <c r="B46" s="90"/>
       <c r="C46" s="7">
         <v>7</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9">
         <f t="shared" si="8"/>
-        <v>14868.566764928002</v>
+        <v>148685.66764928002</v>
       </c>
       <c r="F46" s="35">
         <f t="shared" si="9"/>
-        <v>17296.588961792</v>
+        <v>172965.88961791998</v>
       </c>
       <c r="G46" s="35">
         <f t="shared" si="10"/>
-        <v>17838.303576251281</v>
+        <v>178383.03576251279</v>
       </c>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="91"/>
+      <c r="B47" s="90"/>
       <c r="C47" s="7">
         <v>8</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9">
         <f t="shared" si="8"/>
-        <v>17165.938100226562</v>
+        <v>171659.38100226561</v>
       </c>
       <c r="F47" s="35">
         <f t="shared" si="9"/>
-        <v>21488.45252026368</v>
+        <v>214884.52520263678</v>
       </c>
       <c r="G47" s="35">
         <f t="shared" si="10"/>
-        <v>22441.027237182589</v>
+        <v>224410.27237182588</v>
       </c>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="91"/>
+      <c r="B48" s="90"/>
       <c r="C48" s="7">
         <v>9</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9">
         <f t="shared" si="8"/>
-        <v>19509.256862231094</v>
+        <v>195092.56862231094</v>
       </c>
       <c r="F48" s="35">
         <f t="shared" si="9"/>
-        <v>25847.990621074227</v>
+        <v>258479.90621074225</v>
       </c>
       <c r="G48" s="35">
         <f t="shared" si="10"/>
-        <v>27250.873462855805</v>
+        <v>272508.73462855804</v>
       </c>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="91"/>
+      <c r="B49" s="90"/>
       <c r="C49" s="7">
         <v>10</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="39">
         <f>E19</f>
-        <v>201899.4419994757</v>
+        <v>2018994.419994757</v>
       </c>
       <c r="F49" s="35">
         <f t="shared" si="9"/>
-        <v>225381.91024591718</v>
+        <v>2253819.1024591718</v>
       </c>
       <c r="G49" s="35">
         <f t="shared" si="10"/>
-        <v>230277.1627686843</v>
+        <v>2302771.6276868433</v>
       </c>
     </row>
     <row r="50" spans="2:7">
@@ -3301,15 +3301,15 @@
       <c r="D50" s="38"/>
       <c r="E50" s="43">
         <f>E49</f>
-        <v>201899.4419994757</v>
+        <v>2018994.419994757</v>
       </c>
       <c r="F50" s="43">
         <f>F49</f>
-        <v>225381.91024591718</v>
+        <v>2253819.1024591718</v>
       </c>
       <c r="G50" s="43">
         <f>G49</f>
-        <v>230277.1627686843</v>
+        <v>2302771.6276868433</v>
       </c>
     </row>
     <row r="53" spans="2:7">
@@ -3318,7 +3318,7 @@
       </c>
       <c r="C53" s="73">
         <f>$C$6</f>
-        <v>30800</v>
+        <v>160160</v>
       </c>
       <c r="E53" s="74"/>
     </row>
@@ -3334,7 +3334,7 @@
       </c>
       <c r="C55" s="17">
         <f>E50</f>
-        <v>201899.4419994757</v>
+        <v>2018994.419994757</v>
       </c>
     </row>
     <row r="56" spans="2:7">
@@ -3343,7 +3343,7 @@
       </c>
       <c r="C56" s="17">
         <f>F50</f>
-        <v>225381.91024591718</v>
+        <v>2253819.1024591718</v>
       </c>
     </row>
     <row r="57" spans="2:7">
@@ -3352,7 +3352,7 @@
       </c>
       <c r="C57" s="17">
         <f>G50</f>
-        <v>230277.1627686843</v>
+        <v>2302771.6276868433</v>
       </c>
     </row>
     <row r="58" spans="2:7">
@@ -3367,7 +3367,7 @@
       </c>
       <c r="C59" s="78">
         <f>D20</f>
-        <v>200000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="60" spans="2:7">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="C60" s="78">
         <f>D20+D35</f>
-        <v>221000</v>
+        <v>2210000</v>
       </c>
     </row>
     <row r="61" spans="2:7">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="C61" s="78">
         <f>D20+F35</f>
-        <v>225200</v>
+        <v>2252000</v>
       </c>
     </row>
     <row r="62" spans="2:7">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="C63" s="80">
         <f>E11</f>
-        <v>4040</v>
+        <v>40400</v>
       </c>
     </row>
     <row r="64" spans="2:7">
@@ -3409,7 +3409,7 @@
       </c>
       <c r="C64" s="80">
         <f>E13</f>
-        <v>8243.2160000000003</v>
+        <v>82432.160000000003</v>
       </c>
     </row>
     <row r="65" spans="2:5">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="C65" s="80">
         <f>E16</f>
-        <v>14868.566764928002</v>
+        <v>148685.66764928002</v>
       </c>
     </row>
     <row r="66" spans="2:5">
@@ -3427,7 +3427,7 @@
       </c>
       <c r="C66" s="80">
         <f>E18</f>
-        <v>19509.256862231094</v>
+        <v>195092.56862231094</v>
       </c>
     </row>
     <row r="67" spans="2:5">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="C67" s="80">
         <f>E19</f>
-        <v>201899.4419994757</v>
+        <v>2018994.419994757</v>
       </c>
     </row>
     <row r="68" spans="2:5">
@@ -3456,15 +3456,15 @@
         <v>377</v>
       </c>
       <c r="C69" s="82">
-        <f>(E69*D69/100)*E5</f>
-        <v>3080</v>
+        <f>MIN(100000,(E69*D69/100)*E5)</f>
+        <v>16016</v>
       </c>
       <c r="D69" s="56">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E69" s="74">
         <f>C6</f>
-        <v>30800</v>
+        <v>160160</v>
       </c>
     </row>
     <row r="70" spans="2:5">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="C70" s="82">
         <f>C69*6</f>
-        <v>18480</v>
+        <v>96096</v>
       </c>
     </row>
     <row r="71" spans="2:5">
@@ -3492,23 +3492,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="B40:B49"/>
     <mergeCell ref="I23:M23"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="B10:B19"/>
     <mergeCell ref="D23:G23"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="B40:B49"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Modal Factor'!$B$1:$B$4</xm:f>
@@ -3528,8 +3528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3609,7 +3609,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f>IF(E5=12,0.09,(IF(E5=6,0.52,IF(E5=3,0.27,1))))</f>
+        <f>IF(E5=12,0.09,(IF(E5=2,0.52,IF(E5=4,0.27,1))))</f>
         <v>1</v>
       </c>
       <c r="G5">
@@ -3651,17 +3651,17 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="14.25" customHeight="1">
-      <c r="C8" s="94" t="s">
+      <c r="C8" s="95" t="s">
         <v>350</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="97" t="s">
         <v>386</v>
       </c>
-      <c r="E8" s="99" t="s">
+      <c r="E8" s="98" t="s">
         <v>244</v>
       </c>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
       <c r="O8">
         <v>12.622999999999999</v>
       </c>
@@ -3671,8 +3671,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="30">
-      <c r="C9" s="95"/>
-      <c r="D9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="97"/>
       <c r="E9" s="27" t="s">
         <v>383</v>
       </c>
@@ -3691,7 +3691,7 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="90" t="s">
         <v>387</v>
       </c>
       <c r="C10" s="7">
@@ -3726,7 +3726,7 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="B11" s="91"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="7">
         <v>2</v>
       </c>
@@ -3759,7 +3759,7 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="B12" s="91"/>
+      <c r="B12" s="90"/>
       <c r="C12" s="7">
         <v>3</v>
       </c>
@@ -3785,7 +3785,7 @@
       <c r="M12" s="31"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="B13" s="91"/>
+      <c r="B13" s="90"/>
       <c r="C13" s="7">
         <v>4</v>
       </c>
@@ -3811,7 +3811,7 @@
       <c r="M13" s="31"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="B14" s="91"/>
+      <c r="B14" s="90"/>
       <c r="C14" s="7">
         <v>5</v>
       </c>
@@ -3837,7 +3837,7 @@
       <c r="M14" s="31"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="B15" s="91"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="7">
         <v>6</v>
       </c>
@@ -3863,7 +3863,7 @@
       <c r="M15" s="31"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="B16" s="91"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="7">
         <v>7</v>
       </c>
@@ -3889,7 +3889,7 @@
       <c r="M16" s="31"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17" s="91"/>
+      <c r="B17" s="90"/>
       <c r="C17" s="7">
         <v>8</v>
       </c>
@@ -3917,7 +3917,7 @@
       <c r="O17" s="28"/>
     </row>
     <row r="18" spans="2:15">
-      <c r="B18" s="91"/>
+      <c r="B18" s="90"/>
       <c r="C18" s="7">
         <v>9</v>
       </c>
@@ -3943,7 +3943,7 @@
       <c r="M18" s="31"/>
     </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="91"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="7">
         <v>10</v>
       </c>
@@ -3990,19 +3990,19 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="14.25" customHeight="1">
-      <c r="D23" s="99" t="s">
+      <c r="D23" s="98" t="s">
         <v>352</v>
       </c>
-      <c r="E23" s="99"/>
-      <c r="F23" s="99"/>
-      <c r="G23" s="99"/>
-      <c r="I23" s="98" t="s">
+      <c r="E23" s="98"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="98"/>
+      <c r="I23" s="94" t="s">
         <v>389</v>
       </c>
-      <c r="J23" s="98"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="98"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="94"/>
+      <c r="M23" s="94"/>
     </row>
     <row r="24" spans="2:15" ht="30">
       <c r="C24" s="5" t="s">
@@ -4133,7 +4133,7 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="2:15" ht="14.25" customHeight="1">
-      <c r="B31" s="85" t="s">
+      <c r="B31" s="91" t="s">
         <v>388</v>
       </c>
       <c r="C31" s="7">
@@ -4172,7 +4172,7 @@
       </c>
     </row>
     <row r="32" spans="2:15">
-      <c r="B32" s="86"/>
+      <c r="B32" s="92"/>
       <c r="C32" s="7">
         <v>8</v>
       </c>
@@ -4209,7 +4209,7 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="86"/>
+      <c r="B33" s="92"/>
       <c r="C33" s="7">
         <v>9</v>
       </c>
@@ -4246,7 +4246,7 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="86"/>
+      <c r="B34" s="92"/>
       <c r="C34" s="7">
         <v>10</v>
       </c>
@@ -4283,7 +4283,7 @@
       </c>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="86"/>
+      <c r="B35" s="92"/>
       <c r="C35" s="8"/>
       <c r="D35" s="19">
         <f>SUM(D25:D34)</f>
@@ -4303,22 +4303,22 @@
       </c>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="86"/>
+      <c r="B36" s="92"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="C38" s="94" t="s">
+      <c r="C38" s="95" t="s">
         <v>350</v>
       </c>
-      <c r="D38" s="96"/>
-      <c r="E38" s="97" t="s">
+      <c r="D38" s="97"/>
+      <c r="E38" s="99" t="s">
         <v>355</v>
       </c>
-      <c r="F38" s="97"/>
-      <c r="G38" s="97"/>
+      <c r="F38" s="99"/>
+      <c r="G38" s="99"/>
     </row>
     <row r="39" spans="2:13" ht="30">
-      <c r="C39" s="95"/>
-      <c r="D39" s="96"/>
+      <c r="C39" s="96"/>
+      <c r="D39" s="97"/>
       <c r="E39" s="27" t="s">
         <v>356</v>
       </c>
@@ -4330,7 +4330,7 @@
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="91" t="s">
+      <c r="B40" s="90" t="s">
         <v>359</v>
       </c>
       <c r="C40" s="7">
@@ -4351,7 +4351,7 @@
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="91"/>
+      <c r="B41" s="90"/>
       <c r="C41" s="7">
         <v>2</v>
       </c>
@@ -4370,7 +4370,7 @@
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="91"/>
+      <c r="B42" s="90"/>
       <c r="C42" s="7">
         <v>3</v>
       </c>
@@ -4389,7 +4389,7 @@
       </c>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="91"/>
+      <c r="B43" s="90"/>
       <c r="C43" s="7">
         <v>4</v>
       </c>
@@ -4408,7 +4408,7 @@
       </c>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="91"/>
+      <c r="B44" s="90"/>
       <c r="C44" s="7">
         <v>5</v>
       </c>
@@ -4427,7 +4427,7 @@
       </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="91"/>
+      <c r="B45" s="90"/>
       <c r="C45" s="7">
         <v>6</v>
       </c>
@@ -4446,7 +4446,7 @@
       </c>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="91"/>
+      <c r="B46" s="90"/>
       <c r="C46" s="7">
         <v>7</v>
       </c>
@@ -4465,7 +4465,7 @@
       </c>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="91"/>
+      <c r="B47" s="90"/>
       <c r="C47" s="7">
         <v>8</v>
       </c>
@@ -4484,7 +4484,7 @@
       </c>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="91"/>
+      <c r="B48" s="90"/>
       <c r="C48" s="7">
         <v>9</v>
       </c>
@@ -4503,7 +4503,7 @@
       </c>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="91"/>
+      <c r="B49" s="90"/>
       <c r="C49" s="7">
         <v>10</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>377</v>
       </c>
       <c r="C69" s="24">
-        <f>(E69*D69/100)*E5</f>
+        <f>MIN(100000,(E69*D69/100)*E5)</f>
         <v>13048.2</v>
       </c>
       <c r="D69">
@@ -4718,20 +4718,19 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="B40:B49"/>
     <mergeCell ref="I23:M23"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="B10:B19"/>
     <mergeCell ref="D23:G23"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="B40:B49"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="80" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -39620,7 +39619,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -39645,7 +39644,7 @@
         <v>240</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0.27</v>
@@ -39656,7 +39655,7 @@
         <v>241</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>0.52</v>
@@ -85164,17 +85163,17 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="14.25" customHeight="1">
-      <c r="C8" s="94" t="s">
+      <c r="C8" s="95" t="s">
         <v>350</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="97" t="s">
         <v>386</v>
       </c>
-      <c r="E8" s="99" t="s">
+      <c r="E8" s="98" t="s">
         <v>244</v>
       </c>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
       <c r="O8">
         <v>12.622999999999999</v>
       </c>
@@ -85184,8 +85183,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="30">
-      <c r="C9" s="95"/>
-      <c r="D9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="97"/>
       <c r="E9" s="11" t="s">
         <v>383</v>
       </c>
@@ -85204,7 +85203,7 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="90" t="s">
         <v>387</v>
       </c>
       <c r="C10" s="7">
@@ -85239,7 +85238,7 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="B11" s="91"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="7">
         <v>2</v>
       </c>
@@ -85272,7 +85271,7 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="B12" s="91"/>
+      <c r="B12" s="90"/>
       <c r="C12" s="7">
         <v>3</v>
       </c>
@@ -85298,7 +85297,7 @@
       <c r="M12" s="31"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="B13" s="91"/>
+      <c r="B13" s="90"/>
       <c r="C13" s="7">
         <v>4</v>
       </c>
@@ -85324,7 +85323,7 @@
       <c r="M13" s="31"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="B14" s="91"/>
+      <c r="B14" s="90"/>
       <c r="C14" s="7">
         <v>5</v>
       </c>
@@ -85350,7 +85349,7 @@
       <c r="M14" s="31"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="B15" s="91"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="7">
         <v>6</v>
       </c>
@@ -85376,7 +85375,7 @@
       <c r="M15" s="31"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="B16" s="91"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="7">
         <v>7</v>
       </c>
@@ -85402,7 +85401,7 @@
       <c r="M16" s="31"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17" s="91"/>
+      <c r="B17" s="90"/>
       <c r="C17" s="7">
         <v>8</v>
       </c>
@@ -85430,7 +85429,7 @@
       <c r="O17" s="28"/>
     </row>
     <row r="18" spans="2:15">
-      <c r="B18" s="91"/>
+      <c r="B18" s="90"/>
       <c r="C18" s="7">
         <v>9</v>
       </c>
@@ -85456,7 +85455,7 @@
       <c r="M18" s="31"/>
     </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="91"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="7">
         <v>10</v>
       </c>
@@ -85503,19 +85502,19 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="14.25" customHeight="1">
-      <c r="D23" s="99" t="s">
+      <c r="D23" s="98" t="s">
         <v>352</v>
       </c>
-      <c r="E23" s="99"/>
-      <c r="F23" s="99"/>
-      <c r="G23" s="99"/>
-      <c r="I23" s="98" t="s">
+      <c r="E23" s="98"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="98"/>
+      <c r="I23" s="94" t="s">
         <v>389</v>
       </c>
-      <c r="J23" s="98"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="98"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="94"/>
+      <c r="M23" s="94"/>
     </row>
     <row r="24" spans="2:15" ht="30">
       <c r="C24" s="5" t="s">
@@ -85646,7 +85645,7 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="2:15" ht="14.25" customHeight="1">
-      <c r="B31" s="85" t="s">
+      <c r="B31" s="91" t="s">
         <v>388</v>
       </c>
       <c r="C31" s="7">
@@ -85685,7 +85684,7 @@
       </c>
     </row>
     <row r="32" spans="2:15">
-      <c r="B32" s="86"/>
+      <c r="B32" s="92"/>
       <c r="C32" s="7">
         <v>8</v>
       </c>
@@ -85722,7 +85721,7 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="86"/>
+      <c r="B33" s="92"/>
       <c r="C33" s="7">
         <v>9</v>
       </c>
@@ -85759,7 +85758,7 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="86"/>
+      <c r="B34" s="92"/>
       <c r="C34" s="7">
         <v>10</v>
       </c>
@@ -85796,7 +85795,7 @@
       </c>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="86"/>
+      <c r="B35" s="92"/>
       <c r="C35" s="8"/>
       <c r="D35" s="19">
         <f>SUM(D25:D34)</f>
@@ -85816,22 +85815,22 @@
       </c>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="86"/>
+      <c r="B36" s="92"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="C38" s="94" t="s">
+      <c r="C38" s="95" t="s">
         <v>350</v>
       </c>
-      <c r="D38" s="96"/>
-      <c r="E38" s="97" t="s">
+      <c r="D38" s="97"/>
+      <c r="E38" s="99" t="s">
         <v>355</v>
       </c>
-      <c r="F38" s="97"/>
-      <c r="G38" s="97"/>
+      <c r="F38" s="99"/>
+      <c r="G38" s="99"/>
     </row>
     <row r="39" spans="2:13" ht="30">
-      <c r="C39" s="95"/>
-      <c r="D39" s="96"/>
+      <c r="C39" s="96"/>
+      <c r="D39" s="97"/>
       <c r="E39" s="11" t="s">
         <v>356</v>
       </c>
@@ -85843,7 +85842,7 @@
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="91" t="s">
+      <c r="B40" s="90" t="s">
         <v>359</v>
       </c>
       <c r="C40" s="7">
@@ -85864,7 +85863,7 @@
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="91"/>
+      <c r="B41" s="90"/>
       <c r="C41" s="7">
         <v>2</v>
       </c>
@@ -85883,7 +85882,7 @@
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="91"/>
+      <c r="B42" s="90"/>
       <c r="C42" s="7">
         <v>3</v>
       </c>
@@ -85902,7 +85901,7 @@
       </c>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="91"/>
+      <c r="B43" s="90"/>
       <c r="C43" s="7">
         <v>4</v>
       </c>
@@ -85921,7 +85920,7 @@
       </c>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="91"/>
+      <c r="B44" s="90"/>
       <c r="C44" s="7">
         <v>5</v>
       </c>
@@ -85940,7 +85939,7 @@
       </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="91"/>
+      <c r="B45" s="90"/>
       <c r="C45" s="7">
         <v>6</v>
       </c>
@@ -85959,7 +85958,7 @@
       </c>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="91"/>
+      <c r="B46" s="90"/>
       <c r="C46" s="7">
         <v>7</v>
       </c>
@@ -85978,7 +85977,7 @@
       </c>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="91"/>
+      <c r="B47" s="90"/>
       <c r="C47" s="7">
         <v>8</v>
       </c>
@@ -85997,7 +85996,7 @@
       </c>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="91"/>
+      <c r="B48" s="90"/>
       <c r="C48" s="7">
         <v>9</v>
       </c>
@@ -86016,7 +86015,7 @@
       </c>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="91"/>
+      <c r="B49" s="90"/>
       <c r="C49" s="7">
         <v>10</v>
       </c>
@@ -86214,17 +86213,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="B10:B19"/>
+    <mergeCell ref="D23:G23"/>
     <mergeCell ref="I23:M23"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="E38:G38"/>
     <mergeCell ref="B40:B49"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="B10:B19"/>
-    <mergeCell ref="D23:G23"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>